<commit_message>
updated new schedules for ramping down temperature to outside condition
</commit_message>
<xml_diff>
--- a/notes/climate_chamber/schedule/warm_fall/WarmF16oct.xlsx
+++ b/notes/climate_chamber/schedule/warm_fall/WarmF16oct.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/notes/climate_chamber/schedule/warm_fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5307D027-0C82-6048-9A5C-EA129D2D4C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36DB1BB-0F54-464A-B81E-F57AF4F40A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37580" yWindow="-1980" windowWidth="27240" windowHeight="16260" xr2:uid="{4D476646-5361-4E43-ACF1-036E5CDB58BE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17240" xr2:uid="{4D476646-5361-4E43-ACF1-036E5CDB58BE}"/>
   </bookViews>
   <sheets>
     <sheet name="WarmF4sept" sheetId="1" r:id="rId1"/>
@@ -942,7 +942,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1043,7 +1043,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1087,7 +1087,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1131,7 +1131,7 @@
         <v>0.125</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1175,7 +1175,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1219,7 +1219,7 @@
         <v>0.25</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C8" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -1307,7 +1307,7 @@
         <v>0.31666666666666665</v>
       </c>
       <c r="C9" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C10">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1395,7 +1395,7 @@
         <v>0.375</v>
       </c>
       <c r="C11">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C12">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="C13">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>0.5</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1571,7 +1571,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C15">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1659,7 +1659,7 @@
         <v>0.625</v>
       </c>
       <c r="C17">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1703,7 +1703,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1747,7 +1747,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C19">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1791,7 +1791,7 @@
         <v>0.75</v>
       </c>
       <c r="C20">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1835,7 +1835,7 @@
         <v>0.7631944444444444</v>
       </c>
       <c r="C21" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="C22">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1923,7 +1923,7 @@
         <v>0.79791666666666672</v>
       </c>
       <c r="C23" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
@@ -1967,7 +1967,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="C24">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2011,7 +2011,7 @@
         <v>0.875</v>
       </c>
       <c r="C25">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2055,7 +2055,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C26">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2099,7 +2099,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="C27">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D27">
         <v>0</v>

</xml_diff>